<commit_message>
update Nosql Training lynda
</commit_message>
<xml_diff>
--- a/Reports.xlsx
+++ b/Reports.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>mstest</t>
   </si>
@@ -353,13 +353,31 @@
   </si>
   <si>
     <t>using convention</t>
+  </si>
+  <si>
+    <t>Team Foundation Build 2010 Introduction</t>
+  </si>
+  <si>
+    <t>the build Environment</t>
+  </si>
+  <si>
+    <t>Demo: Installing the Build Service</t>
+  </si>
+  <si>
+    <t>Up and Running Nosql Satabases</t>
+  </si>
+  <si>
+    <t>couchdb Applicatrion</t>
+  </si>
+  <si>
+    <t>Understanding NoSQL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,9 +386,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF555555"/>
       <name val="Lucida Sans Unicode"/>
       <family val="2"/>
     </font>
@@ -407,11 +443,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,18 +733,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -720,10 +762,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -736,28 +778,28 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -770,15 +812,15 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -791,7 +833,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -812,17 +854,17 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -843,70 +885,70 @@
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -943,119 +985,157 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="C50" t="s">
+      <c r="C50" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="C57" t="s">
+      <c r="C57" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="C58" t="s">
+      <c r="C58" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="C59" t="s">
+      <c r="C59" s="3" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="12.75">
+      <c r="B62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>